<commit_message>
Cambiando lógica a formato múltiple
</commit_message>
<xml_diff>
--- a/__src__/__tmp__/tmp_cuadro_final.xlsx
+++ b/__src__/__tmp__/tmp_cuadro_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Desktop\Koening\HuffModel\huff-model-macro\__src__\__tmp__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D066E3-8112-46FB-BCB5-F857E18F5407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8133C2-8AE5-4C51-91AB-DFFC3179BE4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="18">
   <si>
     <t>ZONA</t>
   </si>
@@ -72,6 +72,9 @@
     <t>Z414</t>
   </si>
   <si>
+    <t>Z396"</t>
+  </si>
+  <si>
     <t>Supermercado</t>
   </si>
   <si>
@@ -79,6 +82,9 @@
   </si>
   <si>
     <t>Plaza Vea Los Olivos</t>
+  </si>
+  <si>
+    <t>Plaza Vea Universitaria</t>
   </si>
 </sst>
 </file>
@@ -481,10 +487,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:I9"/>
+      <selection activeCell="A18" sqref="A18:I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,28 +529,28 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>2000</v>
       </c>
       <c r="D2">
-        <v>18000</v>
+        <v>25000</v>
       </c>
       <c r="E2">
-        <v>0.1111111111111111</v>
+        <v>0.08</v>
       </c>
       <c r="F2">
         <v>3.2</v>
       </c>
       <c r="G2">
-        <v>0.27100000000000002</v>
+        <v>0.26400000000000001</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>9702.98</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>0.66227741174109767</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -552,28 +558,28 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3">
         <v>10000</v>
       </c>
       <c r="D3">
-        <v>18000</v>
+        <v>25000</v>
       </c>
       <c r="E3">
-        <v>0.55555555555555558</v>
+        <v>0.4</v>
       </c>
       <c r="F3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G3">
-        <v>0.60599999999999998</v>
+        <v>0.50900000000000001</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>3798.9</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>0.25929411989546058</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -581,173 +587,521 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <v>6000</v>
       </c>
       <c r="D4">
-        <v>18000</v>
+        <v>25000</v>
       </c>
       <c r="E4">
-        <v>0.33333333333333331</v>
+        <v>0.24</v>
       </c>
       <c r="F4">
-        <v>2.4</v>
+        <v>1.2</v>
       </c>
       <c r="G4">
-        <v>1.679</v>
+        <v>1.603</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>706.93</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>4.8251544441206107E-2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C5">
-        <v>2000</v>
+        <v>7000</v>
       </c>
       <c r="D5">
-        <v>2000</v>
+        <v>25000</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="F5">
-        <v>3.2</v>
+        <v>1.6</v>
       </c>
       <c r="G5">
-        <v>0.57099999999999995</v>
+        <v>3.48</v>
       </c>
       <c r="H5">
-        <v>30582.5</v>
+        <v>442.12</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>3.017692392223565E-2</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6">
         <v>2000</v>
       </c>
       <c r="D6">
-        <v>12000</v>
+        <v>25000</v>
       </c>
       <c r="E6">
-        <v>0.16666666666666671</v>
+        <v>0.08</v>
       </c>
       <c r="F6">
         <v>3.2</v>
       </c>
       <c r="G6">
-        <v>0.57799999999999996</v>
+        <v>0.57099999999999995</v>
       </c>
       <c r="H6">
-        <v>693.17</v>
+        <v>16816.150000000001</v>
       </c>
       <c r="I6">
-        <v>0.75205598350873393</v>
+        <v>0.54986202889300384</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7">
         <v>10000</v>
       </c>
       <c r="D7">
-        <v>12000</v>
+        <v>25000</v>
       </c>
       <c r="E7">
-        <v>0.83333333333333337</v>
+        <v>0.4</v>
       </c>
       <c r="F7">
         <v>2</v>
       </c>
       <c r="G7">
-        <v>1.1060000000000001</v>
+        <v>0.90100000000000002</v>
       </c>
       <c r="H7">
-        <v>228.53</v>
+        <v>8029.09</v>
       </c>
       <c r="I7">
-        <v>0.24794401649126621</v>
+        <v>0.26253879262283752</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C8">
-        <v>2000</v>
+        <v>6000</v>
       </c>
       <c r="D8">
-        <v>8000</v>
+        <v>25000</v>
       </c>
       <c r="E8">
-        <v>0.25</v>
+        <v>0.24</v>
       </c>
       <c r="F8">
-        <v>3.2</v>
+        <v>1.2</v>
       </c>
       <c r="G8">
-        <v>1.0960000000000001</v>
+        <v>1.226</v>
       </c>
       <c r="H8">
-        <v>6418.33</v>
+        <v>3896.83</v>
       </c>
       <c r="I8">
-        <v>0.54723752195487951</v>
+        <v>0.12742029834719151</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>7000</v>
+      </c>
+      <c r="D9">
+        <v>25000</v>
+      </c>
+      <c r="E9">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F9">
+        <v>1.6</v>
+      </c>
+      <c r="G9">
+        <v>3.1789999999999998</v>
+      </c>
+      <c r="H9">
+        <v>1840.42</v>
+      </c>
+      <c r="I9">
+        <v>6.0178880136967268E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10">
+        <v>2000</v>
+      </c>
+      <c r="D10">
+        <v>25000</v>
+      </c>
+      <c r="E10">
+        <v>0.08</v>
+      </c>
+      <c r="F10">
+        <v>3.2</v>
+      </c>
+      <c r="G10">
+        <v>0.57799999999999996</v>
+      </c>
+      <c r="H10">
+        <v>615.92999999999995</v>
+      </c>
+      <c r="I10">
+        <v>0.66824706252508925</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <v>10000</v>
+      </c>
+      <c r="D11">
+        <v>25000</v>
+      </c>
+      <c r="E11">
+        <v>0.4</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>1.1060000000000001</v>
+      </c>
+      <c r="H11">
+        <v>202.91</v>
+      </c>
+      <c r="I11">
+        <v>0.22014516496511921</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <v>6000</v>
+      </c>
+      <c r="D12">
+        <v>25000</v>
+      </c>
+      <c r="E12">
+        <v>0.24</v>
+      </c>
+      <c r="F12">
+        <v>1.2</v>
+      </c>
+      <c r="G12">
+        <v>2.0249999999999999</v>
+      </c>
+      <c r="H12">
+        <v>61.33</v>
+      </c>
+      <c r="I12">
+        <v>6.6539367046034012E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13">
+        <v>7000</v>
+      </c>
+      <c r="D13">
+        <v>25000</v>
+      </c>
+      <c r="E13">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F13">
+        <v>1.6</v>
+      </c>
+      <c r="G13">
+        <v>3.968</v>
+      </c>
+      <c r="H13">
+        <v>41.54</v>
+      </c>
+      <c r="I13">
+        <v>4.5068405463757587E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>2000</v>
+      </c>
+      <c r="D14">
+        <v>25000</v>
+      </c>
+      <c r="E14">
+        <v>0.08</v>
+      </c>
+      <c r="F14">
+        <v>3.2</v>
+      </c>
+      <c r="G14">
+        <v>1.0960000000000001</v>
+      </c>
+      <c r="H14">
+        <v>3744.17</v>
+      </c>
+      <c r="I14">
+        <v>0.31923390751333702</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15">
+        <v>6000</v>
+      </c>
+      <c r="D15">
+        <v>25000</v>
+      </c>
+      <c r="E15">
+        <v>0.24</v>
+      </c>
+      <c r="F15">
+        <v>1.2</v>
+      </c>
+      <c r="G15">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="H15">
+        <v>3346.19</v>
+      </c>
+      <c r="I15">
+        <v>0.28530149779044572</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
         <v>15</v>
       </c>
-      <c r="C9">
+      <c r="C16">
+        <v>10000</v>
+      </c>
+      <c r="D16">
+        <v>25000</v>
+      </c>
+      <c r="E16">
+        <v>0.4</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16">
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="H16">
+        <v>3758.41</v>
+      </c>
+      <c r="I16">
+        <v>0.32044803263131783</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17">
+        <v>7000</v>
+      </c>
+      <c r="D17">
+        <v>25000</v>
+      </c>
+      <c r="E17">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F17">
+        <v>1.6</v>
+      </c>
+      <c r="G17">
+        <v>2.327</v>
+      </c>
+      <c r="H17">
+        <v>879.84</v>
+      </c>
+      <c r="I17">
+        <v>7.5016562064899414E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18">
+        <v>2000</v>
+      </c>
+      <c r="D18">
+        <v>25000</v>
+      </c>
+      <c r="E18">
+        <v>0.08</v>
+      </c>
+      <c r="F18">
+        <v>0.8</v>
+      </c>
+      <c r="G18">
+        <v>4.0750000000000002</v>
+      </c>
+      <c r="H18">
+        <v>6.21</v>
+      </c>
+      <c r="I18">
+        <v>0.47695852534562211</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19">
+        <v>10000</v>
+      </c>
+      <c r="D19">
+        <v>25000</v>
+      </c>
+      <c r="E19">
+        <v>0.4</v>
+      </c>
+      <c r="F19">
+        <v>0.5</v>
+      </c>
+      <c r="G19">
+        <v>4.4249999999999998</v>
+      </c>
+      <c r="H19">
+        <v>3.54</v>
+      </c>
+      <c r="I19">
+        <v>0.27188940092165897</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20">
         <v>6000</v>
       </c>
-      <c r="D9">
-        <v>8000</v>
-      </c>
-      <c r="E9">
-        <v>0.75</v>
-      </c>
-      <c r="F9">
-        <v>1.2</v>
-      </c>
-      <c r="G9">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="H9">
-        <v>5310.27</v>
-      </c>
-      <c r="I9">
-        <v>0.45276247804512049</v>
+      <c r="D20">
+        <v>25000</v>
+      </c>
+      <c r="E20">
+        <v>0.24</v>
+      </c>
+      <c r="F20">
+        <v>0.3</v>
+      </c>
+      <c r="G20">
+        <v>5.5460000000000003</v>
+      </c>
+      <c r="H20">
+        <v>1.66</v>
+      </c>
+      <c r="I20">
+        <v>0.12749615975422429</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21">
+        <v>7000</v>
+      </c>
+      <c r="D21">
+        <v>25000</v>
+      </c>
+      <c r="E21">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F21">
+        <v>0.4</v>
+      </c>
+      <c r="G21">
+        <v>7.4260000000000002</v>
+      </c>
+      <c r="H21">
+        <v>1.61</v>
+      </c>
+      <c r="I21">
+        <v>0.1236559139784946</v>
       </c>
     </row>
   </sheetData>

</xml_diff>